<commit_message>
Đăng ký dựa trên môn học chính, phụ, đặc biệt
</commit_message>
<xml_diff>
--- a/userNtools.xlsx
+++ b/userNtools.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">list!$A$1:$I$72</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1085,7 +1085,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1299,13 +1299,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1642,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,71 +1692,73 @@
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
-        <f t="shared" ref="A2:A33" si="0">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>308</v>
+      <c r="F2" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="30"/>
+        <v>68</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>314</v>
+        <v>37</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>321</v>
+        <v>229</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>320</v>
+        <v>123</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="30"/>
+        <v>68</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>239</v>
+        <v>325</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>169</v>
+        <v>324</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>290</v>
@@ -1765,248 +1767,250 @@
         <v>309</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I4" s="30"/>
+        <v>147</v>
+      </c>
+      <c r="I4" s="29"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>103</v>
+        <v>75</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>279</v>
+      <c r="B6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>262</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>102</v>
+        <v>75</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>254</v>
+        <v>188</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>308</v>
+      <c r="F7" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>137</v>
+        <v>75</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>306</v>
+      <c r="F9" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>88</v>
+        <v>178</v>
       </c>
       <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>306</v>
+      <c r="F10" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>205</v>
+        <v>72</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>315</v>
+        <v>13</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>317</v>
+        <v>241</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>316</v>
+        <v>240</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H11" s="21"/>
+        <v>72</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>306</v>
+      <c r="F12" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>204</v>
+        <v>72</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>237</v>
+      <c r="B13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>235</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>236</v>
+        <v>167</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>290</v>
@@ -2018,23 +2022,25 @@
         <v>72</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="I13" s="30"/>
+        <v>172</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>290</v>
@@ -2046,99 +2052,97 @@
         <v>72</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>226</v>
+        <v>267</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>303</v>
+      <c r="F15" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>118</v>
+        <v>307</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>240</v>
+        <v>132</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>309</v>
+      <c r="F16" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>72</v>
+        <v>307</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>218</v>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>265</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>311</v>
+      <c r="F17" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>67</v>
+        <v>307</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="I17" s="31" t="s">
-        <v>210</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2166,7 +2170,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -2194,45 +2198,45 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>308</v>
+      <c r="F20" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>260</v>
+        <v>179</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>290</v>
@@ -2244,189 +2248,189 @@
         <v>74</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>299</v>
+        <v>52</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>282</v>
+        <v>180</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G22" s="13"/>
+        <v>304</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="H22" s="19" t="s">
-        <v>294</v>
+        <v>182</v>
       </c>
       <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>309</v>
+      <c r="F23" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>96</v>
+        <v>254</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>310</v>
+      <c r="F24" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="I24" s="30"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>309</v>
+      <c r="F25" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>313</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>264</v>
+        <v>319</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>304</v>
+      <c r="F26" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>191</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H26" s="19"/>
       <c r="I26" s="30"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>310</v>
+      <c r="F27" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="I27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>313</v>
+        <v>21</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>319</v>
+        <v>249</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>318</v>
+        <v>107</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>290</v>
@@ -2437,134 +2441,136 @@
       <c r="G28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="19"/>
+      <c r="H28" s="19" t="s">
+        <v>141</v>
+      </c>
       <c r="I28" s="30"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
-        <f t="shared" si="0"/>
+      <c r="A29" s="15">
+        <f>ROW()-1</f>
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>146</v>
+      <c r="B29" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="I29" s="30"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
-        <f t="shared" si="0"/>
+      <c r="A30" s="15">
+        <f>ROW()-1</f>
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>160</v>
+      <c r="B30" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>195</v>
       </c>
       <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>303</v>
+      <c r="F31" s="13" t="s">
+        <v>308</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>114</v>
+        <v>73</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="I31" s="30"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>308</v>
+      <c r="F32" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>307</v>
+        <v>69</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="I32" s="30"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>325</v>
+        <v>234</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>324</v>
+        <v>130</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>290</v>
@@ -2573,138 +2579,138 @@
         <v>309</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I33" s="29"/>
+        <v>146</v>
+      </c>
+      <c r="I33" s="30"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
-        <f t="shared" ref="A34:A65" si="1">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>33</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>262</v>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>186</v>
+        <v>127</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>187</v>
+        <v>69</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="I35" s="29"/>
+        <v>69</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="I35" s="30"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>323</v>
+        <v>269</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>322</v>
+        <v>202</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>311</v>
+      <c r="F36" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>165</v>
+        <v>305</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>205</v>
       </c>
       <c r="I36" s="30"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="H37" s="19" t="s">
-        <v>135</v>
+        <v>305</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>204</v>
       </c>
       <c r="I37" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>37</v>
       </c>
-      <c r="B38" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>245</v>
+      <c r="B38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>273</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>81</v>
+        <v>199</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>290</v>
@@ -2713,28 +2719,26 @@
         <v>306</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="I38" s="31" t="s">
-        <v>210</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="I38" s="30"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>290</v>
@@ -2743,500 +2747,504 @@
         <v>306</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>84</v>
+        <v>305</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>207</v>
       </c>
       <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>231</v>
+        <v>270</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>309</v>
+      <c r="F40" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>143</v>
+        <v>305</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>225</v>
+        <v>272</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>115</v>
+        <v>201</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>303</v>
+      <c r="F41" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>116</v>
+        <v>305</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>308</v>
+      <c r="F42" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="I42" s="30"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F43" s="13" t="s">
-        <v>308</v>
+      <c r="F43" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="I43" s="30"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>300</v>
+        <v>31</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>284</v>
+        <v>89</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="G44" s="13"/>
+        <v>310</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="H44" s="19" t="s">
-        <v>293</v>
+        <v>97</v>
       </c>
       <c r="I44" s="30"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>122</v>
+        <v>76</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="I45" s="30"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
-        <f t="shared" si="1"/>
+      <c r="A46" s="13">
+        <f>ROW()-1</f>
         <v>45</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H46" s="25" t="s">
-        <v>193</v>
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="I46" s="30"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>199</v>
+        <v>92</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F47" s="13" t="s">
-        <v>306</v>
+      <c r="F47" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>209</v>
+        <v>76</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <f t="shared" si="1"/>
+      <c r="A48" s="13">
+        <f>ROW()-1</f>
         <v>47</v>
       </c>
-      <c r="B48" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E48" s="28" t="s">
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H48" s="21" t="s">
-        <v>112</v>
+        <v>76</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="I48" s="30"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>232</v>
+        <v>278</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="I49" s="30"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>303</v>
+      <c r="F50" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>120</v>
+        <v>71</v>
+      </c>
+      <c r="H50" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="I50" s="30"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>214</v>
+      <c r="B51" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>245</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>311</v>
+      <c r="F51" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I51" s="30"/>
+        <v>82</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>311</v>
+      <c r="F52" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="I52" s="30"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="E53" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>311</v>
+      <c r="F53" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>164</v>
+        <v>86</v>
       </c>
       <c r="I53" s="30"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
-        <f t="shared" si="1"/>
+      <c r="A54" s="13">
+        <f>ROW()-1</f>
         <v>53</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H54" s="25" t="s">
-        <v>195</v>
+      <c r="B54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>24</v>
+        <v>314</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>247</v>
+        <v>321</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>85</v>
+        <v>320</v>
       </c>
       <c r="E55" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F55" s="13" t="s">
-        <v>306</v>
+      <c r="F55" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H55" s="19" t="s">
-        <v>86</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="H55" s="19"/>
       <c r="I55" s="30"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>55</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>244</v>
+      <c r="B56" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>218</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F56" s="13" t="s">
-        <v>306</v>
+      <c r="F56" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="I56" s="30"/>
+        <v>161</v>
+      </c>
+      <c r="I56" s="31" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>290</v>
@@ -3248,107 +3256,107 @@
         <v>67</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I57" s="30"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>256</v>
+        <v>323</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>110</v>
+        <v>322</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>308</v>
+      <c r="F58" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="I58" s="30"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="I59" s="30"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F60" s="13" t="s">
-        <v>308</v>
+      <c r="F60" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>307</v>
+        <v>67</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="I60" s="30"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>60</v>
       </c>
-      <c r="B61" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>216</v>
+      <c r="B61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>221</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>290</v>
@@ -3360,111 +3368,109 @@
         <v>67</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="I61" s="31" t="s">
-        <v>210</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="I61" s="30"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>61</v>
       </c>
-      <c r="B62" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>235</v>
+      <c r="B62" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>215</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="I62" s="31" t="s">
-        <v>210</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="I62" s="30"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>62</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>277</v>
+      <c r="B63" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>216</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="I63" s="30"/>
+        <v>159</v>
+      </c>
+      <c r="I63" s="31" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H64" s="19" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="I64" s="30"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
-        <f t="shared" si="1"/>
+        <f>ROW()-1</f>
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>290</v>
@@ -3476,51 +3482,49 @@
         <v>67</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I65" s="30"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
-        <f t="shared" ref="A66:A74" si="2">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>60</v>
+        <v>315</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>220</v>
+        <v>317</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>154</v>
+        <v>316</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="H66" s="19" t="s">
-        <v>163</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="H66" s="21"/>
       <c r="I66" s="30"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>290</v>
@@ -3529,206 +3533,202 @@
         <v>303</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>68</v>
+        <v>312</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="I67" s="29"/>
+        <v>118</v>
+      </c>
+      <c r="I67" s="30"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>271</v>
+        <v>224</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F68" s="13" t="s">
-        <v>306</v>
+      <c r="F68" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H68" s="20" t="s">
-        <v>207</v>
+        <v>312</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="I68" s="30"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F69" s="13" t="s">
-        <v>306</v>
+      <c r="F69" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H69" s="20" t="s">
-        <v>206</v>
+        <v>312</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>116</v>
       </c>
       <c r="I69" s="30"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>275</v>
+        <v>228</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>290</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>98</v>
+        <v>312</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="I70" s="30"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
-        <f t="shared" si="2"/>
+      <c r="A71" s="1">
+        <f>ROW()-1</f>
         <v>70</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E71" s="18" t="s">
+      <c r="B71" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" s="28" t="s">
         <v>290</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>101</v>
+        <v>312</v>
+      </c>
+      <c r="H71" s="21" t="s">
+        <v>112</v>
       </c>
       <c r="I71" s="30"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>201</v>
+        <v>119</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="F72" s="13" t="s">
-        <v>306</v>
+      <c r="F72" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="H72" s="20" t="s">
-        <v>208</v>
+        <v>312</v>
+      </c>
+      <c r="H72" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="I72" s="30"/>
     </row>
     <row r="73" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>41</v>
+        <v>299</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>188</v>
+        <v>282</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="G73" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>189</v>
+        <v>292</v>
+      </c>
+      <c r="G73" s="13"/>
+      <c r="H73" s="19" t="s">
+        <v>294</v>
       </c>
       <c r="I73" s="30"/>
     </row>
     <row r="74" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
-        <f t="shared" si="2"/>
+        <f>ROW()-1</f>
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>171</v>
+        <v>284</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G74" s="13" t="s">
-        <v>72</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="G74" s="13"/>
       <c r="H74" s="19" t="s">
-        <v>177</v>
+        <v>293</v>
       </c>
       <c r="I74" s="30"/>
     </row>
@@ -3743,11 +3743,11 @@
   </sheetData>
   <autoFilter ref="A1:I72">
     <sortState ref="A2:I74">
-      <sortCondition ref="B1:B72"/>
+      <sortCondition ref="G1:G72"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D36" r:id="rId1"/>
+    <hyperlink ref="D58" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId2"/>

</xml_diff>